<commit_message>
Complete COMP - 512 All Assignment
</commit_message>
<xml_diff>
--- a/03.COMP 513 - Computational Mathematics and Models I/08.COMP_513_Assignment_8_ex2007.xlsx
+++ b/03.COMP 513 - Computational Mathematics and Models I/08.COMP_513_Assignment_8_ex2007.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$160</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -342,6 +345,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -359,18 +374,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -385,6 +388,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Histogram</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -463,11 +484,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="0"/>
-        <c:axId val="74962816"/>
+        <c:axId val="74700672"/>
         <c:axId val="75301248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74962816"/>
+        <c:axId val="74700672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,7 +550,7 @@
         <c:spPr>
           <a:noFill/>
         </c:spPr>
-        <c:crossAx val="74962816"/>
+        <c:crossAx val="74700672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -538,11 +559,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -558,7 +574,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -568,6 +584,29 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cumulative Frequency</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Curve</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -575,6 +614,22 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$F$8:$F$14</c:f>
@@ -638,7 +693,7 @@
         </c:ser>
         <c:marker val="1"/>
         <c:axId val="75308416"/>
-        <c:axId val="75326976"/>
+        <c:axId val="75331072"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="75308416"/>
@@ -666,14 +721,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75326976"/>
+        <c:crossAx val="75331072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75326976"/>
+        <c:axId val="75331072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -726,7 +781,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -736,6 +791,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Histogram</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -754,7 +827,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$F$63:$F$69</c:f>
+              <c:f>Sheet1!$F$66:$F$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -784,7 +857,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$63:$G$69</c:f>
+              <c:f>Sheet1!$G$66:$G$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -855,7 +928,6 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -898,7 +970,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -907,20 +979,36 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:style val="1"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Line Graph</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$F$63:$F$69</c:f>
+              <c:f>Sheet1!$F$66:$F$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -950,7 +1038,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$63:$G$69</c:f>
+              <c:f>Sheet1!$G$66:$G$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -980,14 +1068,25 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$F$63:$F$69</c:f>
+              <c:f>Sheet1!$F$66:$F$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1017,7 +1116,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$63:$G$69</c:f>
+              <c:f>Sheet1!$G$66:$G$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1047,11 +1146,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75381376"/>
-        <c:axId val="75395840"/>
+        <c:axId val="76823168"/>
+        <c:axId val="76837632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75381376"/>
+        <c:axId val="76823168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1076,14 +1175,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75395840"/>
+        <c:crossAx val="76837632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75395840"/>
+        <c:axId val="76837632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1208,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75381376"/>
+        <c:crossAx val="76823168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1131,8 +1230,8 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1141,6 +1240,29 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cumulative Frequency</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Curve</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1148,9 +1270,23 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$F$63:$F$69</c:f>
+              <c:f>Sheet1!$F$66:$F$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1180,7 +1316,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$63:$H$69</c:f>
+              <c:f>Sheet1!$H$66:$H$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1210,11 +1346,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75423744"/>
-        <c:axId val="75425664"/>
+        <c:axId val="76861440"/>
+        <c:axId val="76863360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75423744"/>
+        <c:axId val="76861440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,14 +1375,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75425664"/>
+        <c:crossAx val="76863360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75425664"/>
+        <c:axId val="76863360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1272,7 +1408,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75423744"/>
+        <c:crossAx val="76861440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1294,7 +1430,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1304,16 +1440,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>196849</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>168274</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1335,15 +1471,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>201179</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>619126</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>75334</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1366,14 +1502,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1394,16 +1530,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>123</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>577273</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1424,16 +1560,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>125</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342901</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>173181</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>895350</xdr:colOff>
-      <xdr:row>144</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:colOff>591705</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>27131</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1740,9 +1876,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="66" zoomScaleSheetLayoutView="66" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="66" zoomScaleSheetLayoutView="66" workbookViewId="0">
+      <selection activeCell="J66" sqref="J66"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
@@ -1770,62 +1908,62 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" customHeight="1">
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="24.75" customHeight="1">
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="20.25" customHeight="1">
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="23.25" customHeight="1">
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="23.25" customHeight="1">
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="26"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="30"/>
       <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1842,7 +1980,7 @@
       <c r="C8" s="19">
         <v>19</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="22" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="20">
@@ -1865,7 +2003,7 @@
       <c r="C9" s="19">
         <v>27</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="23" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="20">
@@ -1888,7 +2026,7 @@
       <c r="C10" s="19">
         <v>35</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="23" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="20">
@@ -1911,7 +2049,7 @@
       <c r="C11" s="19">
         <v>43</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="23" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="21">
@@ -1934,7 +2072,7 @@
       <c r="C12" s="19">
         <v>51</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="24" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="20">
@@ -1957,7 +2095,7 @@
       <c r="C13" s="19">
         <v>59</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="22" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="20">
@@ -1980,7 +2118,7 @@
       <c r="C14" s="19">
         <v>67</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="23" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="20">
@@ -2103,202 +2241,202 @@
     <row r="40" spans="11:11">
       <c r="K40" s="2"/>
     </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="1">
+    <row r="60" spans="1:10">
+      <c r="A60" s="1">
         <v>2</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="22" t="s">
+      <c r="C60" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
-      <c r="H57" s="22"/>
-      <c r="I57" s="22"/>
-      <c r="J57" s="22"/>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="B59" s="10" t="s">
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="26"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="B62" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="22" t="s">
+      <c r="C62" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="22"/>
-    </row>
-    <row r="62" spans="1:10" ht="24.75" customHeight="1">
-      <c r="B62" s="1" t="s">
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="B65" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C62" s="23" t="s">
+      <c r="C65" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D62" s="24"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="4" t="s">
+      <c r="D65" s="28"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G62" s="14" t="s">
+      <c r="G65" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H62" s="14" t="s">
+      <c r="H65" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
-      <c r="C63" s="15">
+    <row r="66" spans="2:8">
+      <c r="C66" s="15">
         <v>118</v>
       </c>
-      <c r="D63" s="28" t="s">
+      <c r="D66" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E63" s="16">
+      <c r="E66" s="16">
         <v>126</v>
       </c>
-      <c r="F63" s="6">
-        <f>MEDIAN(C63:E63)</f>
+      <c r="F66" s="6">
+        <f>MEDIAN(C66:E66)</f>
         <v>122</v>
       </c>
-      <c r="G63" s="8">
+      <c r="G66" s="8">
         <v>6</v>
       </c>
-      <c r="H63" s="8">
+      <c r="H66" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
-      <c r="C64" s="11">
+    <row r="67" spans="2:8">
+      <c r="C67" s="11">
         <v>127</v>
       </c>
-      <c r="D64" s="30" t="s">
+      <c r="D67" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E64" s="17">
+      <c r="E67" s="17">
         <v>135</v>
       </c>
-      <c r="F64" s="7">
-        <f t="shared" ref="F64:F69" si="1">MEDIAN(C64:E64)</f>
+      <c r="F67" s="7">
+        <f t="shared" ref="F67:F72" si="1">MEDIAN(C67:E67)</f>
         <v>131</v>
       </c>
-      <c r="G64" s="8">
+      <c r="G67" s="8">
         <v>10</v>
       </c>
-      <c r="H64" s="8">
+      <c r="H67" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="3:8">
-      <c r="C65" s="11">
+    <row r="68" spans="2:8">
+      <c r="C68" s="11">
         <v>136</v>
       </c>
-      <c r="D65" s="30" t="s">
+      <c r="D68" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E65" s="17">
+      <c r="E68" s="17">
         <v>144</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F68" s="7">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="G65" s="8">
+      <c r="G68" s="8">
         <v>18</v>
       </c>
-      <c r="H65" s="8">
+      <c r="H68" s="7">
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="3:8">
-      <c r="C66" s="11">
+    <row r="69" spans="2:8">
+      <c r="C69" s="11">
         <v>145</v>
       </c>
-      <c r="D66" s="30" t="s">
+      <c r="D69" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E66" s="17">
+      <c r="E69" s="17">
         <v>153</v>
       </c>
-      <c r="F66" s="7">
+      <c r="F69" s="7">
         <f t="shared" si="1"/>
         <v>149</v>
       </c>
-      <c r="G66" s="8">
+      <c r="G69" s="8">
         <v>24</v>
       </c>
-      <c r="H66" s="8">
+      <c r="H69" s="7">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="3:8">
-      <c r="C67" s="11">
+    <row r="70" spans="2:8">
+      <c r="C70" s="11">
         <v>154</v>
       </c>
-      <c r="D67" s="30" t="s">
+      <c r="D70" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E67" s="17">
+      <c r="E70" s="17">
         <v>162</v>
       </c>
-      <c r="F67" s="7">
+      <c r="F70" s="7">
         <f t="shared" si="1"/>
         <v>158</v>
       </c>
-      <c r="G67" s="8">
+      <c r="G70" s="8">
         <v>10</v>
       </c>
-      <c r="H67" s="8">
+      <c r="H70" s="7">
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="3:8">
-      <c r="C68" s="11">
+    <row r="71" spans="2:8">
+      <c r="C71" s="11">
         <v>163</v>
       </c>
-      <c r="D68" s="30" t="s">
+      <c r="D71" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E68" s="17">
+      <c r="E71" s="17">
         <v>171</v>
       </c>
-      <c r="F68" s="7">
+      <c r="F71" s="7">
         <f t="shared" si="1"/>
         <v>167</v>
       </c>
-      <c r="G68" s="8">
+      <c r="G71" s="8">
         <v>8</v>
       </c>
-      <c r="H68" s="8">
+      <c r="H71" s="7">
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="3:8">
-      <c r="C69" s="12">
+    <row r="72" spans="2:8">
+      <c r="C72" s="12">
         <v>172</v>
       </c>
-      <c r="D69" s="31" t="s">
+      <c r="D72" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E69" s="18">
+      <c r="E72" s="18">
         <v>180</v>
       </c>
-      <c r="F69" s="5">
+      <c r="F72" s="5">
         <f t="shared" si="1"/>
         <v>176</v>
       </c>
-      <c r="G69" s="13">
+      <c r="G72" s="13">
         <v>4</v>
       </c>
-      <c r="H69" s="13">
+      <c r="H72" s="5">
         <v>80</v>
       </c>
     </row>
@@ -2307,9 +2445,9 @@
     <sortCondition ref="K1"/>
   </sortState>
   <mergeCells count="8">
-    <mergeCell ref="C57:J57"/>
-    <mergeCell ref="C59:J59"/>
-    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C60:J60"/>
+    <mergeCell ref="C62:J62"/>
+    <mergeCell ref="C65:E65"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C4:I4"/>
@@ -2317,10 +2455,10 @@
     <mergeCell ref="C7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="63" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="54" max="16383" man="1"/>
-    <brk id="98" max="16383" man="1"/>
+    <brk id="58" max="9" man="1"/>
+    <brk id="134" max="9" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>